<commit_message>
finalised comments of AE
</commit_message>
<xml_diff>
--- a/literature_table/table.xlsx
+++ b/literature_table/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Documents/1-research/1-research_papers/3.under review/Work with Rob Hyndman/forecasting-emergency-medcine/literature_table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbsbr11/Documents/1.Research/1.Research papers/1.under review/forecasting-emergency-medicine/literature_table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E9C74-347B-1943-926B-A7808622C88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B4B363-0D93-3342-A1B3-2495EFD5D020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="760" windowWidth="20960" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Reference</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Stationary,  Exponential Smoothing State Space (ETS), Poisson regression using Generalized Linear Model (GLM) and tscount (TSGLM), a simple empirical distribution and an ensemble method</t>
+  </si>
+  <si>
+    <t>Reproducibility</t>
   </si>
 </sst>
 </file>
@@ -221,9 +224,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,10 +473,11 @@
     <col min="6" max="6" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="13.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +502,11 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -510,7 +519,7 @@
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -522,9 +531,12 @@
       <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1">
@@ -548,8 +560,11 @@
       <c r="H3" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -574,8 +589,11 @@
       <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -600,8 +618,11 @@
       <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -626,8 +647,11 @@
       <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -652,8 +676,11 @@
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -678,8 +705,11 @@
       <c r="H8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="D9" s="3"/>
@@ -687,13 +717,13 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>

</xml_diff>